<commit_message>
Se cambian los log y se guardan archivos excel exportados de los reportes
</commit_message>
<xml_diff>
--- a/cypress/cypress/downloads/Tablero_ Solicitudes a la Dirección Jurídica-Exportado.xlsx
+++ b/cypress/cypress/downloads/Tablero_ Solicitudes a la Dirección Jurídica-Exportado.xlsx
@@ -378,7 +378,7 @@
       </x:c>
       <x:c r="B6" t="inlineStr">
         <x:is>
-          <x:t>76</x:t>
+          <x:t>77</x:t>
         </x:is>
       </x:c>
       <x:c r="C6" t="inlineStr">
@@ -661,355 +661,355 @@
     <x:row>
       <x:c r="A10" t="inlineStr">
         <x:is>
+          <x:t>ANALISTA2 PRUEBAS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B10" t="inlineStr">
+        <x:is>
+          <x:t>0</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C10" t="inlineStr">
+        <x:is>
+          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D10" t="inlineStr">
+        <x:is>
+          <x:t>DIRECCIÓN JURÍDICA</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E10" t="inlineStr">
+        <x:is>
+          <x:t>RESPUESTA A DERECHOS DE PETICIÓN</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F10" t="inlineStr">
+        <x:is>
+          <x:t>5</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G10" t="inlineStr">
+        <x:is>
+          <x:t>2023-65-I</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H10" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+      <x:c r="I10" t="inlineStr">
+        <x:is>
+          <x:t>3/01/2023 4:54:52 p. m.</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="J10" t="inlineStr">
+        <x:is>
+          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="K10" t="inlineStr">
+        <x:is>
+          <x:t>DIRECCIÓN JURÍDICA</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="L10" t="inlineStr">
+        <x:is>
+          <x:t>331290</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="M10" t="inlineStr">
+        <x:is>
+          <x:t>CIERRE CON OBSERVACIONES</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="N10" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c r="A11" t="inlineStr">
+        <x:is>
+          <x:t>ANALISTA2 PRUEBAS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B11" t="inlineStr">
+        <x:is>
+          <x:t>0</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C11" t="inlineStr">
+        <x:is>
+          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D11" t="inlineStr">
+        <x:is>
+          <x:t>VICERRECTORÍA ADMINISTRATIVA</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E11" t="inlineStr">
+        <x:is>
+          <x:t>CONCEPTOS JURÍDICOS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F11" t="inlineStr">
+        <x:is>
+          <x:t>30</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G11" t="inlineStr">
+        <x:is>
+          <x:t>2023-225-I</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H11" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+      <x:c r="I11" t="inlineStr">
+        <x:is>
+          <x:t>19/01/2023 9:44:29 a. m.</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="J11" t="inlineStr">
+        <x:is>
+          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="K11" t="inlineStr">
+        <x:is>
+          <x:t>DIVISIÓN DE SERVICIOS LOGÍSTICOS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="L11" t="inlineStr">
+        <x:is>
+          <x:t>334014</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="M11" t="inlineStr">
+        <x:is>
+          <x:t>CERRADO</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="N11" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c r="A12" t="inlineStr">
+        <x:is>
+          <x:t>SIN ASIGNAR</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B12" t="inlineStr">
+        <x:is>
+          <x:t>0</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C12" t="inlineStr">
+        <x:is>
+          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D12" t="inlineStr">
+        <x:is>
+          <x:t>VICERRECTORÍA ADMINISTRATIVA</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E12" t="inlineStr">
+        <x:is>
+          <x:t>CONCEPTOS JURÍDICOS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F12" t="inlineStr">
+        <x:is>
+          <x:t>30</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G12" t="inlineStr">
+        <x:is>
+          <x:t>2023-249-I</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H12" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+      <x:c r="I12" t="inlineStr">
+        <x:is>
+          <x:t>19/01/2023 12:36:36 p. m.</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="J12" t="inlineStr">
+        <x:is>
+          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="K12" t="inlineStr">
+        <x:is>
+          <x:t>DIVISIÓN DE SERVICIOS LOGÍSTICOS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="L12" t="inlineStr">
+        <x:is>
+          <x:t>334177</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="M12" t="inlineStr">
+        <x:is>
+          <x:t>CERRADO</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="N12" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c r="A13" t="inlineStr">
+        <x:is>
           <x:t>ANALISTA3 PRUEBAS</x:t>
         </x:is>
       </x:c>
-      <x:c r="B10" t="inlineStr">
-        <x:is>
-          <x:t>26</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C10" t="inlineStr">
-        <x:is>
-          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D10" t="inlineStr">
+      <x:c r="B13" t="inlineStr">
+        <x:is>
+          <x:t>27</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C13" t="inlineStr">
+        <x:is>
+          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D13" t="inlineStr">
         <x:is>
           <x:t>SECRETARÍA GENERAL</x:t>
         </x:is>
       </x:c>
-      <x:c r="E10" t="inlineStr">
+      <x:c r="E13" t="inlineStr">
         <x:is>
           <x:t>CONCEPTOS JURÍDICOS</x:t>
         </x:is>
       </x:c>
-      <x:c r="F10" t="inlineStr">
+      <x:c r="F13" t="inlineStr">
         <x:is>
           <x:t>30</x:t>
         </x:is>
       </x:c>
-      <x:c r="G10" t="inlineStr">
+      <x:c r="G13" t="inlineStr">
         <x:is>
           <x:t>2023-488-I</x:t>
         </x:is>
       </x:c>
-      <x:c r="H10" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-      <x:c r="I10" t="inlineStr">
+      <x:c r="H13" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+      <x:c r="I13" t="inlineStr">
         <x:is>
           <x:t>13/03/2023 5:23:05 p. m.</x:t>
         </x:is>
       </x:c>
-      <x:c r="J10" t="inlineStr">
-        <x:is>
-          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="K10" t="inlineStr">
+      <x:c r="J13" t="inlineStr">
+        <x:is>
+          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="K13" t="inlineStr">
         <x:is>
           <x:t>DIVISIÓN DE GESTIÓN DOCUMENTAL</x:t>
         </x:is>
       </x:c>
-      <x:c r="L10" t="inlineStr">
+      <x:c r="L13" t="inlineStr">
         <x:is>
           <x:t>353039</x:t>
         </x:is>
       </x:c>
-      <x:c r="M10" t="inlineStr">
+      <x:c r="M13" t="inlineStr">
         <x:is>
           <x:t>ASIGNADO</x:t>
         </x:is>
       </x:c>
-      <x:c r="N10" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c r="A11" t="inlineStr">
+      <x:c r="N13" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c r="A14" t="inlineStr">
         <x:is>
           <x:t>ANALISTA3 PRUEBAS</x:t>
         </x:is>
       </x:c>
-      <x:c r="B11" t="inlineStr">
-        <x:is>
-          <x:t>26</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C11" t="inlineStr">
-        <x:is>
-          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D11" t="inlineStr">
+      <x:c r="B14" t="inlineStr">
+        <x:is>
+          <x:t>27</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C14" t="inlineStr">
+        <x:is>
+          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D14" t="inlineStr">
         <x:is>
           <x:t>SECRETARÍA GENERAL</x:t>
         </x:is>
       </x:c>
-      <x:c r="E11" t="inlineStr">
+      <x:c r="E14" t="inlineStr">
         <x:is>
           <x:t>RESPUESTA A DERECHOS DE PETICIÓN</x:t>
         </x:is>
       </x:c>
-      <x:c r="F11" t="inlineStr">
+      <x:c r="F14" t="inlineStr">
         <x:is>
           <x:t>5</x:t>
         </x:is>
       </x:c>
-      <x:c r="G11" t="inlineStr">
+      <x:c r="G14" t="inlineStr">
         <x:is>
           <x:t>2023-489-I</x:t>
         </x:is>
       </x:c>
-      <x:c r="H11" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-      <x:c r="I11" t="inlineStr">
+      <x:c r="H14" t="inlineStr">
+        <x:is>
+          <x:t/>
+        </x:is>
+      </x:c>
+      <x:c r="I14" t="inlineStr">
         <x:is>
           <x:t>13/03/2023 5:24:05 p. m.</x:t>
         </x:is>
       </x:c>
-      <x:c r="J11" t="inlineStr">
-        <x:is>
-          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="K11" t="inlineStr">
+      <x:c r="J14" t="inlineStr">
+        <x:is>
+          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="K14" t="inlineStr">
         <x:is>
           <x:t>DIVISIÓN DE GESTIÓN DOCUMENTAL</x:t>
         </x:is>
       </x:c>
-      <x:c r="L11" t="inlineStr">
+      <x:c r="L14" t="inlineStr">
         <x:is>
           <x:t>353040</x:t>
         </x:is>
       </x:c>
-      <x:c r="M11" t="inlineStr">
+      <x:c r="M14" t="inlineStr">
         <x:is>
           <x:t>ASIGNADO</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="N11" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c r="A12" t="inlineStr">
-        <x:is>
-          <x:t>ANALISTA2 PRUEBAS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B12" t="inlineStr">
-        <x:is>
-          <x:t>0</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C12" t="inlineStr">
-        <x:is>
-          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D12" t="inlineStr">
-        <x:is>
-          <x:t>DIRECCIÓN JURÍDICA</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E12" t="inlineStr">
-        <x:is>
-          <x:t>RESPUESTA A DERECHOS DE PETICIÓN</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F12" t="inlineStr">
-        <x:is>
-          <x:t>5</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="G12" t="inlineStr">
-        <x:is>
-          <x:t>2023-65-I</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="H12" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-      <x:c r="I12" t="inlineStr">
-        <x:is>
-          <x:t>3/01/2023 4:54:52 p. m.</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J12" t="inlineStr">
-        <x:is>
-          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="K12" t="inlineStr">
-        <x:is>
-          <x:t>DIRECCIÓN JURÍDICA</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="L12" t="inlineStr">
-        <x:is>
-          <x:t>331290</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M12" t="inlineStr">
-        <x:is>
-          <x:t>CIERRE CON OBSERVACIONES</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="N12" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c r="A13" t="inlineStr">
-        <x:is>
-          <x:t>ANALISTA2 PRUEBAS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B13" t="inlineStr">
-        <x:is>
-          <x:t>0</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C13" t="inlineStr">
-        <x:is>
-          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D13" t="inlineStr">
-        <x:is>
-          <x:t>VICERRECTORÍA ADMINISTRATIVA</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E13" t="inlineStr">
-        <x:is>
-          <x:t>CONCEPTOS JURÍDICOS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F13" t="inlineStr">
-        <x:is>
-          <x:t>30</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="G13" t="inlineStr">
-        <x:is>
-          <x:t>2023-225-I</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="H13" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-      <x:c r="I13" t="inlineStr">
-        <x:is>
-          <x:t>19/01/2023 9:44:29 a. m.</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J13" t="inlineStr">
-        <x:is>
-          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="K13" t="inlineStr">
-        <x:is>
-          <x:t>DIVISIÓN DE SERVICIOS LOGÍSTICOS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="L13" t="inlineStr">
-        <x:is>
-          <x:t>334014</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M13" t="inlineStr">
-        <x:is>
-          <x:t>CERRADO</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="N13" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c r="A14" t="inlineStr">
-        <x:is>
-          <x:t>SIN ASIGNAR</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B14" t="inlineStr">
-        <x:is>
-          <x:t>0</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C14" t="inlineStr">
-        <x:is>
-          <x:t>UNIDAD DE ASESORÍA JURÍDICA INSTITUCIONAL</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D14" t="inlineStr">
-        <x:is>
-          <x:t>VICERRECTORÍA ADMINISTRATIVA</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E14" t="inlineStr">
-        <x:is>
-          <x:t>CONCEPTOS JURÍDICOS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F14" t="inlineStr">
-        <x:is>
-          <x:t>30</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="G14" t="inlineStr">
-        <x:is>
-          <x:t>2023-249-I</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="H14" t="inlineStr">
-        <x:is>
-          <x:t/>
-        </x:is>
-      </x:c>
-      <x:c r="I14" t="inlineStr">
-        <x:is>
-          <x:t>19/01/2023 12:36:36 p. m.</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J14" t="inlineStr">
-        <x:is>
-          <x:t>NO REFERIDO A ASUNTOS CONTRACTUALES</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="K14" t="inlineStr">
-        <x:is>
-          <x:t>DIVISIÓN DE SERVICIOS LOGÍSTICOS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="L14" t="inlineStr">
-        <x:is>
-          <x:t>334177</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M14" t="inlineStr">
-        <x:is>
-          <x:t>CERRADO</x:t>
         </x:is>
       </x:c>
       <x:c r="N14" t="inlineStr">

</xml_diff>